<commit_message>
modified documentation and test cases
</commit_message>
<xml_diff>
--- a/SRIP/test_cases.xlsx
+++ b/SRIP/test_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>Click on 'start' after the simulation stops moving.</t>
+  </si>
+  <si>
+    <t>Simulation in chrome browser</t>
+  </si>
+  <si>
+    <t>Version 75.0.3770.100</t>
+  </si>
+  <si>
+    <t>Open animaton in browser.</t>
+  </si>
+  <si>
+    <t>Animation is viewed.</t>
   </si>
 </sst>
 </file>
@@ -457,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="53.25" customHeight="1"/>
@@ -499,13 +511,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>32</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="53.25" customHeight="1">
@@ -513,16 +528,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="53.25" customHeight="1">
@@ -530,13 +542,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
@@ -544,13 +559,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="53.25" customHeight="1">
@@ -558,13 +573,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="53.25" customHeight="1">
@@ -572,13 +587,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="53.25" customHeight="1">
@@ -586,13 +601,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="53.25" customHeight="1">
@@ -600,12 +615,26 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="53.25" customHeight="1">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>